<commit_message>
Fix incorrect external import
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2899219-4A2E-2A4B-9B0E-8E1AFC83AF34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E0E77E-6932-0C4F-9C6F-CF4A96F577E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5380" yWindow="2080" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5360" yWindow="2080" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>psychiatric facility [NCIT:C53536]; transportation [NCIT:C141286]; public transportation [NCIT:C141287]</t>
   </si>
   <si>
-    <t>environment [ENVO:01000254]; rural area [ENVO:01000772]; urban area [ENVO:01000856]; research facility [ENVO:00000469]; park [ENVO:00000562]; forest [ENVO:00000111]; beach [ENVO:00000091]; grassland [ENVO:00000106]; road [ENVO:00000064]</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/gaz</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]</t>
+  </si>
+  <si>
+    <t>environment [ENVO:01000254]; rural area [ENVO:01000772]; urban area [ENVO:00000856]; research facility [ENVO:00000469]; park [ENVO:00000562]; forest [ENVO:00000111]; beach [ENVO:00000091]; grassland [ENVO:00000106]; road [ENVO:00000064]</t>
   </si>
 </sst>
 </file>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -580,7 +580,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -700,7 +700,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>31</v>
@@ -714,13 +714,13 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -728,7 +728,7 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -742,10 +742,10 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Bug fix for relationship problem
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E0E77E-6932-0C4F-9C6F-CF4A96F577E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DEC83E-D3DF-024A-B841-F8A4598206C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5360" yWindow="2080" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Ontology ID</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>environment [ENVO:01000254]; rural area [ENVO:01000772]; urban area [ENVO:00000856]; research facility [ENVO:00000469]; park [ENVO:00000562]; forest [ENVO:00000111]; beach [ENVO:00000091]; grassland [ENVO:00000106]; road [ENVO:00000064]</t>
+  </si>
+  <si>
+    <t>Intermediates</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,7 +561,7 @@
     <col min="4" max="4" width="54" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -568,8 +574,11 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -582,8 +591,11 @@
       <c r="D2" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -596,8 +608,11 @@
       <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -610,8 +625,11 @@
       <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -624,8 +642,11 @@
       <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -638,8 +659,11 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -652,8 +676,11 @@
       <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -666,8 +693,11 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -680,8 +710,11 @@
       <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -694,8 +727,11 @@
       <c r="D10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -708,8 +744,11 @@
       <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -722,8 +761,11 @@
       <c r="D12" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -736,8 +778,11 @@
       <c r="D13" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -749,6 +794,9 @@
       </c>
       <c r="D14" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Build OWL file for Behaviour module
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7481E78A-5485-914C-A1F9-C5842B1C3623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C0A15-9DAD-F44F-9EB8-A82F67C73A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="1220" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15020" yWindow="-13600" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
     <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]; has role [RO:0000087]</t>
   </si>
   <si>
-    <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]</t>
+    <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; function [BFO:0000034]</t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Release Mechanism of Action ontology
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101C0A15-9DAD-F44F-9EB8-A82F67C73A02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2430A760-F580-E745-B996-85890A265D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15020" yWindow="-13600" windowWidth="19940" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17180" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Imports" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Ontology ID</t>
   </si>
@@ -102,9 +102,6 @@
     <t>MF</t>
   </si>
   <si>
-    <t>person [MF:0000016]</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/mf.owl</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>facility [OMRSE:00000062]; residential facility [OMRSE:00000191]; healthcare facility [OMRSE:00000102]; hospital facility [OMRSE:00000063]; emergency department facility [OMRSE:00000114]; hospice facility [OMRSE:00000104]; rehabilitation facility [OMRSE:00000106]; school facility [OMRSE:00000064]</t>
   </si>
   <si>
-    <t>environment [ENVO:01000254]; rural area [ENVO:01000772]; urban area [ENVO:00000856]; research facility [ENVO:00000469]; park [ENVO:00000562]; forest [ENVO:00000111]; beach [ENVO:00000091]; grassland [ENVO:00000106]; road [ENVO:00000064]</t>
-  </si>
-  <si>
     <t>Intermediates</t>
   </si>
   <si>
@@ -156,17 +150,62 @@
     <t>Prefix</t>
   </si>
   <si>
-    <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]; has role [RO:0000087]</t>
-  </si>
-  <si>
     <t>process [BFO:0000015]; object aggregate [BFO:0000027]; role [BFO:0000023]; disposition [BFO:0000016]; object [BFO:0000030]; process profile [BFO:0000144]; site [BFO:0000029]; function [BFO:0000034]</t>
+  </si>
+  <si>
+    <t>ADDICTO</t>
+  </si>
+  <si>
+    <t>MFOEM</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/mfoem.owl</t>
+  </si>
+  <si>
+    <t>UBERON</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/uberon.owl</t>
+  </si>
+  <si>
+    <t>bodily feeling [MFOEM:000202];appraisal of pleasantness [MFOEM:000061];anger [MFOEM:000009];disgust [MFOEM:000019 ];appraisal [MFOEM:000005];appraisal of goal importance [MFOEM:000072];animal-nature disgust [MFOEM:000021];appraisal of avoidability of consequences [MFOEM:000091];appraisal of expectedness [MFOEM:000060];affective process [MFOEM:000195];appraisal of dangerousness [MFOEM:000103];anxiety [MFOEM:000028];appraisal of desirability of consequences [MFOEM:000085];emotion process [MFOEM:000001 ];appraisal as caused by an other [MFOEM:000078];appraisal of causal agency [MFOEM:000075];core disgust [MFOEM:000020];emotional action tendency [MFOEM:000007 ];appraisal as caused by self [MFOEM:000076];appraisal process [MFOEM:000002]</t>
+  </si>
+  <si>
+    <t>anatomical structure [UBERON:0000061]</t>
+  </si>
+  <si>
+    <t>addiction [ADDICTO:0000349]</t>
+  </si>
+  <si>
+    <t>OGMS</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ogms.owl</t>
+  </si>
+  <si>
+    <t>bodily process [OGMS:0000060]</t>
+  </si>
+  <si>
+    <t>environment [ENVO:01000254]; rural area [ENVO:01000772]; urban area [ENVO:00000856]; research facility [ENVO:00000469]; park [ENVO:00000562]; forest [ENVO:00000111]; beach [ENVO:00000091]; grassland [ENVO:00000106]; road [ENVO:00000064];﻿ecosystem [ENVO:01001110];﻿environmental disposition [ENVO:01000452]</t>
+  </si>
+  <si>
+    <t>arousal [MF:0000012];cognitive representation [MF:0000031];cognitive process [MF:0000008];attending [MF:0000018];belief [MF:0000041];bodily disposition [MF:0000032];bodily quality [MF:0000074 ];consciousness [MF:0000017];person [MF:0000016]</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/addicto-org/addiction-ontology/master/addicto.owl</t>
+  </si>
+  <si>
+    <t>"ADDICTO: http://addictovocab.org/ADDICTO_"</t>
+  </si>
+  <si>
+    <t>has part [BFO:0000051]; bearer of [RO:0000053]; inheres in [RO:0000052]; located in [RO:0001025]; participates in [RO:0000056]; has participant [RO:0000057]; has disposition [RO:0000091]; has role [RO:0000087]; is part of [BFO:0000050]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,6 +226,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCDBE97"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -224,6 +269,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,15 +584,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="54" style="1" customWidth="1"/>
@@ -566,13 +612,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -583,10 +629,10 @@
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -600,10 +646,10 @@
         <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -617,10 +663,10 @@
         <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -634,10 +680,10 @@
         <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -654,7 +700,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -668,10 +714,10 @@
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -688,10 +734,10 @@
         <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -702,47 +748,47 @@
         <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>30</v>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -753,30 +799,102 @@
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="255" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed IRI of external ontology gaz
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/HBCP/ontologies/Upper Level BCIO/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD47A61-4B3F-FD45-8E47-8EC8747DDC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479D623-4DEE-8E45-8C80-394505008D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -118,9 +131,6 @@
     <t>GAZ</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/gaz</t>
-  </si>
-  <si>
     <t>geographic location [GAZ:00000448]</t>
   </si>
   <si>
@@ -206,13 +216,16 @@
   </si>
   <si>
     <t>has occurrent part [BFO:0000117]; has profile [BFO:0000119];process profile of [BFO:0000133]</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/gaz.owl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,6 +238,14 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,14 +265,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,7 +579,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -631,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -726,14 +750,14 @@
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -741,16 +765,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -758,16 +782,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -775,36 +799,36 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
         <v>42</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>46</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -812,16 +836,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
         <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>49</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -829,16 +853,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -846,16 +870,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
         <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -863,22 +887,25 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>57</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>59</v>
       </c>
-      <c r="E18" t="s">
-        <v>60</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{421C846E-E525-7747-B833-730F0C5C8B3D}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed "Curation status" mapping to "has curation status"
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/ontologies/Upper Level BCIO/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D67B5B-25AF-B946-8611-F0B107BB4112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C887E5-0AB2-8E4B-8C77-06EA6A1AE492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>http://purl.obolibrary.org/obo/iao.owl</t>
   </si>
   <si>
-    <t>is about [IAO:0000136]; data item [IAO:0000027]; report [IAO:0000088]; plan specification [IAO:0000104]; information content entity [IAO:0000030];curation status specification [IAO:0000078]</t>
-  </si>
-  <si>
     <t>OBI</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t>has output [RO:0002234]; realizes [BFO:0000055]; realized in [BFO:0000054]; output of [RO:0002353]; temporally related to [RO:0002222]; causal relation between entities [RO:0002506]</t>
+  </si>
+  <si>
+    <t>is about [IAO:0000136]; data item [IAO:0000027]; report [IAO:0000088]; plan specification [IAO:0000104]; information content entity [IAO:0000030];curation status specification [IAO:0000078]; has curation status [IAO:0000114]</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -627,7 +627,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -644,7 +644,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -661,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -678,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -686,16 +686,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -703,16 +703,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -720,16 +720,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -737,16 +737,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -754,16 +754,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -771,16 +771,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -788,36 +788,36 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
         <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -825,16 +825,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -842,16 +842,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -859,16 +859,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -876,19 +876,19 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>55</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>56</v>
-      </c>
-      <c r="E18" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imported personal attribute [BCIO:050300]
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,7 +484,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,7 +511,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -540,7 +538,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -568,7 +565,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -596,7 +592,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -624,7 +619,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -652,7 +646,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -680,7 +673,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -708,7 +700,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -736,7 +727,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -796,7 +786,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -824,7 +813,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -852,7 +840,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -880,7 +867,6 @@
           <t>all</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -908,7 +894,28 @@
           <t>minimal</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>bcio</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>personal attribute [BCIO:050300]</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updating MF and MFOEM
</commit_message>
<xml_diff>
--- a/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
+++ b/Upper Level BCIO/inputs/BCIO_External_Imports.xlsx
@@ -843,7 +843,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://raw.githubusercontent.com/jannahastings/emotion-ontology/247c3e33cf00189b0c688c76b5b008d324a43d24/ontology/MFOEM.owl</t>
+          <t>https://raw.githubusercontent.com/jannahastings/emotion-ontology/e3a12f2527e13aa1e4f85e6aa63c5763ea49709c/ontology/MFOEM.owl</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://raw.githubusercontent.com/jannahastings/mental-functioning-ontology/62aaff35a50acba4e11e735605dcf62647f9d27d/ontology/MF.owl</t>
+          <t>https://raw.githubusercontent.com/jannahastings/mental-functioning-ontology/29c0274bb98f6d2de0c078f85d4da18f11e562fd/ontology/MF.owl</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">

</xml_diff>